<commit_message>
N236 P1_8 and P1_9 are re-assigned as VCOM pins to enable UART printf output
</commit_message>
<xml_diff>
--- a/docs/r01lib_pin_table.xlsx
+++ b/docs/r01lib_pin_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedd/Desktop/dl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB4D715-4630-C242-AF9C-01A4DE395FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E27794-1FB3-4D41-98E7-7C89278904C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24600" yWindow="3460" windowWidth="37620" windowHeight="32540" activeTab="4" xr2:uid="{F4A4BD97-1D13-3141-8799-357F4902D58A}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="317">
   <si>
     <t>FRDM-MCXN947</t>
     <phoneticPr fontId="1"/>
@@ -1149,6 +1149,10 @@
   </si>
   <si>
     <t>"r01lib pin names" tables are updated to clarify the pins which have multiple names</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>N236 P1_8 and P1_9 are re-assigned as VCOM pins to enable UART printf output</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3683,11 +3687,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="I16:I19"/>
     <mergeCell ref="A48:A79"/>
     <mergeCell ref="C45:N45"/>
     <mergeCell ref="C46:D46"/>
@@ -3696,6 +3695,11 @@
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="K46:L46"/>
     <mergeCell ref="M46:N46"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="I16:I19"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3707,8 +3711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF8339D-3246-D248-B338-467DAA04C626}">
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I42" sqref="A3:I42"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.7109375" defaultRowHeight="14"/>
@@ -4937,11 +4941,11 @@
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
-      <c r="E57" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>171</v>
+      <c r="E57" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>274</v>
@@ -4968,11 +4972,11 @@
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>171</v>
+      <c r="F58" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>275</v>
@@ -5631,12 +5635,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="I16:I19"/>
     <mergeCell ref="A49:A80"/>
     <mergeCell ref="C46:N46"/>
     <mergeCell ref="C47:D47"/>
@@ -5645,6 +5643,12 @@
     <mergeCell ref="I47:J47"/>
     <mergeCell ref="K47:L47"/>
     <mergeCell ref="M47:N47"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="I16:I19"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7378,12 +7382,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="I30:I33"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
     <mergeCell ref="A48:A79"/>
     <mergeCell ref="C45:L45"/>
     <mergeCell ref="C46:D46"/>
@@ -7391,6 +7389,12 @@
     <mergeCell ref="G46:H46"/>
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="K46:L46"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="I30:I33"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8988,6 +8992,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A50:A81"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="H40:H41"/>
     <mergeCell ref="G38:G39"/>
@@ -8995,12 +9005,6 @@
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="G20:G21"/>
     <mergeCell ref="H20:H21"/>
-    <mergeCell ref="A50:A81"/>
-    <mergeCell ref="C47:J47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9012,7 +9016,7 @@
   <dimension ref="B2:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -9084,8 +9088,12 @@
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="11">
+        <v>45637</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" s="11"/>
@@ -9158,15 +9166,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002C98D15B0064474782E8EDBA35A51CC2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="84bc66ae19ca557e54d7014d86ef62c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6946600b-d432-4ec1-a6de-e6a1f3354bfd" xmlns:ns3="43135f08-7c27-4a7c-bc6d-152a25501e39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f294aa8e50c0a16a8ee0b06cd98abedc" ns2:_="" ns3:_="">
     <xsd:import namespace="6946600b-d432-4ec1-a6de-e6a1f3354bfd"/>
@@ -9373,6 +9372,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -9385,14 +9393,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{993051E6-CE55-49FB-9812-9A2B302725FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02F2913-AEC8-45FD-9F40-2703FA5F6AAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9411,6 +9411,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{993051E6-CE55-49FB-9812-9A2B302725FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D7A352-4E74-4D3B-B371-7F84A478DD81}">
   <ds:schemaRefs>

</xml_diff>